<commit_message>
File di checklist aggiornato
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/report-checklist.xlsx
+++ b/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/costaa/Clienti/Salutis/FSE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/costaa/Clienti/Salutis/FSE/it-fse-accreditamento/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC14583-1AF7-6F49-B73F-E28277363507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81DC2A7-4256-1446-848F-D83EDC738922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54400" yWindow="-5820" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-5820" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="572">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4639,10 +4639,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="N153" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I220" sqref="I220"/>
+      <selection pane="bottomRight" activeCell="P172" sqref="P172:S172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11556,10 +11556,18 @@
         <v>307</v>
       </c>
       <c r="O172" s="34"/>
-      <c r="P172" s="34"/>
-      <c r="Q172" s="34"/>
-      <c r="R172" s="34"/>
-      <c r="S172" s="34"/>
+      <c r="P172" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q172" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="R172" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="S172" s="74" t="s">
+        <v>495</v>
+      </c>
       <c r="T172" s="74" t="s">
         <v>305</v>
       </c>
@@ -17469,7 +17477,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J34 M34:N34 P34:R34 J36:J40 M36:N40 P36:R40 J42 M42:N42 P42:R42 J44:J48 M44:N48 P44:R48 J10:J32 M10:N32 P10:R32 M197:N219 P197:R219 M50:N50 J50 P50:R50 J52:J149 M52:N149 P52:R149 P172:R195 M173:N195 J173:J195 J197:J219</xm:sqref>
+          <xm:sqref>J34 M34:N34 P34:R34 J36:J40 M36:N40 P36:R40 J42 M42:N42 P42:R42 J44:J48 M44:N48 P44:R48 J10:J32 M10:N32 P10:R32 M197:N219 P197:R219 M50:N50 J50 P50:R50 J52:J149 M52:N149 P52:R149 J197:J219 M173:N195 J173:J195 P173:R195</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -19728,27 +19736,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -20006,10 +19993,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20032,20 +20051,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modifica report list - test 149
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/report-checklist.xlsx
+++ b/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/costaa/Clienti/Salutis/FSE/it-fse-accreditamento/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0FD4D5-F256-FE44-ABC1-AACB72FA8212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32396C0E-3FCC-DD47-AC26-B3128A61A165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-5820" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4648,10 +4648,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F150" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I220" sqref="I220"/>
+      <selection pane="bottomRight" activeCell="A152" sqref="A152:XFD152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10314,6 +10314,9 @@
       </c>
       <c r="E152" s="31" t="s">
         <v>452</v>
+      </c>
+      <c r="F152" s="32">
+        <v>45716</v>
       </c>
       <c r="G152" s="33" t="s">
         <v>568</v>
@@ -19753,15 +19756,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20023,27 +20023,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20068,9 +20062,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Corretti 148, 149 e 374
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/report-checklist.xlsx
+++ b/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/costaa/Clienti/Salutis/FSE/it-fse-accreditamento/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7D0220-BA6C-2F49-BF2D-B4E2B5D712E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694A233D-6AA2-104D-B05A-93F03770C04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="573">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2148,46 +2148,40 @@
     <t>20/02/2025T08:39:35</t>
   </si>
   <si>
-    <t>ba61ed1c00e8f72d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.e681f9ecb1ccad05edb23f4c98320d091eeee432aed80b37f5b54e49a3393d42.847e61b627^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>28/02/2025T10:27:37Z</t>
   </si>
   <si>
-    <t>28/02/2025T10:29:45Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.e681f9ecb1ccad05edb23f4c98320d091eeee432aed80b37f5b54e49a3393d42.58a31d2e33^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>28/02/2025T10:30:53Z</t>
-  </si>
-  <si>
-    <t>072e78aa2b4b0812</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.e681f9ecb1ccad05edb23f4c98320d091eeee432aed80b37f5b54e49a3393d42.d986f04d54^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>28/02/2025T10:31:40Z</t>
   </si>
   <si>
-    <t>c21fe34566e0d749</t>
-  </si>
-  <si>
-    <t>28/02/2025T10:32:35Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.e681f9ecb1ccad05edb23f4c98320d091eeee432aed80b37f5b54e49a3393d42.7ec9eb0e9a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.e681f9ecb1ccad05edb23f4c98320d091eeee432aed80b37f5b54e49a3393d42.124c2c5cd4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>62d2ab31a731f99b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.7ea73d015c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f91ed66fdf4afb02</t>
+  </si>
+  <si>
+    <t>31/03/2025T09:18:06Z</t>
+  </si>
+  <si>
+    <t>83ceec89776109ac</t>
+  </si>
+  <si>
+    <t>31/03/2025T09:23:46Z</t>
+  </si>
+  <si>
+    <t>7a17fa6e56d51c2e</t>
+  </si>
+  <si>
+    <t>31/03/2025T09:26:44Z</t>
   </si>
 </sst>
 </file>
@@ -4648,10 +4642,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E165" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H150" sqref="H150"/>
+      <selection pane="bottomRight" activeCell="G220" sqref="G220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10217,13 +10211,13 @@
         <v>45716</v>
       </c>
       <c r="G150" s="33" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H150" s="33" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="I150" s="33" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="J150" s="74" t="s">
         <v>87</v>
@@ -10265,16 +10259,16 @@
         <v>451</v>
       </c>
       <c r="F151" s="32">
-        <v>45716</v>
+        <v>45747</v>
       </c>
       <c r="G151" s="33" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="H151" s="33" t="s">
-        <v>561</v>
+        <v>567</v>
       </c>
       <c r="I151" s="33" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="J151" s="74" t="s">
         <v>87</v>
@@ -10316,16 +10310,16 @@
         <v>452</v>
       </c>
       <c r="F152" s="32">
-        <v>45716</v>
+        <v>45747</v>
       </c>
       <c r="G152" s="33" t="s">
+        <v>570</v>
+      </c>
+      <c r="H152" s="33" t="s">
+        <v>569</v>
+      </c>
+      <c r="I152" s="33" t="s">
         <v>566</v>
-      </c>
-      <c r="H152" s="33" t="s">
-        <v>567</v>
-      </c>
-      <c r="I152" s="33" t="s">
-        <v>565</v>
       </c>
       <c r="J152" s="74" t="s">
         <v>87</v>
@@ -10370,13 +10364,13 @@
         <v>45716</v>
       </c>
       <c r="G153" s="33" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="H153" s="33" t="s">
         <v>515</v>
       </c>
       <c r="I153" s="33" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="J153" s="74" t="s">
         <v>87</v>
@@ -12472,16 +12466,16 @@
         <v>482</v>
       </c>
       <c r="F196" s="32">
-        <v>45716</v>
+        <v>45747</v>
       </c>
       <c r="G196" s="33" t="s">
+        <v>572</v>
+      </c>
+      <c r="H196" s="33" t="s">
         <v>571</v>
       </c>
-      <c r="H196" s="33" t="s">
-        <v>570</v>
-      </c>
       <c r="I196" s="33" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="J196" s="74" t="s">
         <v>87</v>
@@ -19756,27 +19750,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -20034,10 +20007,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20060,20 +20065,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiornati test 149 e 374
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/report-checklist.xlsx
+++ b/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/costaa/Clienti/Salutis/FSE/it-fse-accreditamento/GATEWAY/S1#111#TECHNOLOGYHEALTHSYSTEMSGROUPSRLXX/ths/salutis/1.2.7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A99C2C1-AEF2-864D-8653-D774CED5996C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DD5D35-BC27-BE40-BAF8-6F4737F9FBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="575">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2163,21 +2163,6 @@
     <t>62d2ab31a731f99b</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.7ea73d015c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>83ceec89776109ac</t>
-  </si>
-  <si>
-    <t>31/03/2025T09:23:46Z</t>
-  </si>
-  <si>
-    <t>7a17fa6e56d51c2e</t>
-  </si>
-  <si>
-    <t>31/03/2025T09:26:44Z</t>
-  </si>
-  <si>
     <t>50c491c405701913</t>
   </si>
   <si>
@@ -2185,6 +2170,24 @@
   </si>
   <si>
     <t>01/04/2025T11:59:07Z</t>
+  </si>
+  <si>
+    <t>18b3c9d88a33cee0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.e681f9ecb1ccad05edb23f4c98320d091eeee432aed80b37f5b54e49a3393d42.68e95e5553^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>04/04/2025T15:12:30Z</t>
+  </si>
+  <si>
+    <t>342fdb32110ddb31</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.e681f9ecb1ccad05edb23f4c98320d091eeee432aed80b37f5b54e49a3393d42.32f4851efe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>04/04/2025T15:16:03Z</t>
   </si>
 </sst>
 </file>
@@ -4645,10 +4648,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E192" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G152" sqref="G152"/>
+      <selection pane="bottomRight" activeCell="G220" sqref="G220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10265,13 +10268,13 @@
         <v>45748</v>
       </c>
       <c r="G151" s="33" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="H151" s="33" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="I151" s="33" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="J151" s="74" t="s">
         <v>87</v>
@@ -10313,16 +10316,16 @@
         <v>452</v>
       </c>
       <c r="F152" s="32">
-        <v>45747</v>
+        <v>45751</v>
       </c>
       <c r="G152" s="33" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="H152" s="33" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="I152" s="33" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="J152" s="74" t="s">
         <v>87</v>
@@ -12469,16 +12472,16 @@
         <v>482</v>
       </c>
       <c r="F196" s="32">
-        <v>45747</v>
+        <v>45751</v>
       </c>
       <c r="G196" s="33" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="H196" s="33" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="I196" s="33" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="J196" s="74" t="s">
         <v>87</v>
@@ -19753,15 +19756,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20023,27 +20023,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20068,9 +20062,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>